<commit_message>
Fix one-line missing in claculation. Wrong name for charts
</commit_message>
<xml_diff>
--- a/collect-earth/collect-earth-app/resources/Uncertainty_Analysis_CollectEarth_Template.xlsx
+++ b/collect-earth/collect-earth-app/resources/Uncertainty_Analysis_CollectEarth_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfonso Sanchez-Paus\workspace\maven.1480939002496\collect-earth\collect-earth-app\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE835994-5B37-48F2-B0D8-447B9844721A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07318F3A-61EB-4895-BADA-FA6DF7FEE978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2382F439-AEE3-43F9-9073-EB2AC7886E33}"/>
   </bookViews>
@@ -1147,19 +1147,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1175,29 +1184,20 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1452,7 +1452,13 @@
             <c:separator>, </c:separator>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1832,7 +1838,13 @@
             <c:separator>, </c:separator>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2212,7 +2224,13 @@
             <c:separator>, </c:separator>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2592,7 +2610,13 @@
             <c:separator>, </c:separator>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2796,7 +2820,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
-              <a:t>Changes from Forest to Other Land Use - FOREST LOSS </a:t>
+              <a:t>Changes from Other Land Use to Forest - FOREST GAIN </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3253,7 +3277,7 @@
                 <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
-              <a:t>Changes from Other Land Use to Forest - FOREST GAIN</a:t>
+              <a:t>Changes from Forest to Other Land Use - FOREST LOSS </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3262,7 +3286,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7083239636588547E-2"/>
+          <c:x val="0.1744053890970475"/>
           <c:y val="3.2098601006911205E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3306,7 +3330,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="397D20"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3347,7 +3371,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="449328"/>
+              <a:srgbClr val="C00000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3388,7 +3412,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="4EA72E"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3429,7 +3453,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="92C089"/>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3470,7 +3497,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="BCD5B7"/>
+              <a:srgbClr val="FFFF00"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3804,6 +3831,11 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3892,6 +3924,11 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3980,6 +4017,11 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -4068,6 +4110,11 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -6269,8 +6316,8 @@
   </sheetPr>
   <dimension ref="A1:AM105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="17" zoomScaleNormal="39" workbookViewId="0">
+      <selection activeCell="AK33" sqref="AK33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6317,94 +6364,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="129"/>
-      <c r="R1" s="129"/>
-      <c r="S1" s="129"/>
-      <c r="T1" s="129"/>
-      <c r="U1" s="129"/>
-      <c r="V1" s="129"/>
-      <c r="W1" s="129"/>
-      <c r="X1" s="129"/>
-      <c r="Y1" s="129"/>
-      <c r="Z1" s="129"/>
-      <c r="AA1" s="129"/>
-      <c r="AB1" s="129"/>
-      <c r="AC1" s="129"/>
-      <c r="AD1" s="129"/>
-      <c r="AE1" s="129"/>
-      <c r="AF1" s="129"/>
-      <c r="AG1" s="129"/>
-      <c r="AH1" s="129"/>
-      <c r="AI1" s="129"/>
-      <c r="AJ1" s="129"/>
-      <c r="AK1" s="129"/>
+      <c r="A1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="122"/>
+      <c r="X1" s="122"/>
+      <c r="Y1" s="122"/>
+      <c r="Z1" s="122"/>
+      <c r="AA1" s="122"/>
+      <c r="AB1" s="122"/>
+      <c r="AC1" s="122"/>
+      <c r="AD1" s="122"/>
+      <c r="AE1" s="122"/>
+      <c r="AF1" s="122"/>
+      <c r="AG1" s="122"/>
+      <c r="AH1" s="122"/>
+      <c r="AI1" s="122"/>
+      <c r="AJ1" s="122"/>
+      <c r="AK1" s="122"/>
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:39" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130" t="s">
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="130"/>
-      <c r="O2" s="130"/>
-      <c r="P2" s="130"/>
-      <c r="Q2" s="130"/>
-      <c r="R2" s="130"/>
-      <c r="S2" s="130"/>
-      <c r="T2" s="130" t="s">
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="130"/>
-      <c r="V2" s="130"/>
-      <c r="W2" s="130"/>
-      <c r="X2" s="130"/>
-      <c r="Y2" s="130"/>
-      <c r="Z2" s="130"/>
-      <c r="AA2" s="130"/>
-      <c r="AB2" s="130"/>
-      <c r="AC2" s="131" t="s">
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
+      <c r="AA2" s="123"/>
+      <c r="AB2" s="123"/>
+      <c r="AC2" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="131"/>
-      <c r="AE2" s="131"/>
-      <c r="AF2" s="131"/>
-      <c r="AG2" s="131"/>
-      <c r="AH2" s="131"/>
-      <c r="AI2" s="131"/>
-      <c r="AJ2" s="131"/>
-      <c r="AK2" s="131"/>
+      <c r="AD2" s="124"/>
+      <c r="AE2" s="124"/>
+      <c r="AF2" s="124"/>
+      <c r="AG2" s="124"/>
+      <c r="AH2" s="124"/>
+      <c r="AI2" s="124"/>
+      <c r="AJ2" s="124"/>
+      <c r="AK2" s="124"/>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
     </row>
@@ -6450,42 +6497,42 @@
       <c r="AM3" s="1"/>
     </row>
     <row r="4" spans="1:39" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="133" t="s">
+      <c r="E4" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="132" t="s">
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="132"/>
-      <c r="N4" s="132"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="132"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="14"/>
       <c r="S4" s="15"/>
-      <c r="T4" s="134" t="s">
+      <c r="T4" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="134"/>
-      <c r="V4" s="134"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="134"/>
-      <c r="Y4" s="134"/>
-      <c r="Z4" s="134"/>
-      <c r="AA4" s="134"/>
-      <c r="AB4" s="134"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="121"/>
+      <c r="Y4" s="121"/>
+      <c r="Z4" s="121"/>
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
@@ -6579,7 +6626,7 @@
       <c r="AM5" s="1"/>
     </row>
     <row r="6" spans="1:39" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="135" t="s">
+      <c r="A6" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B6" s="27">
@@ -6612,16 +6659,16 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="124" t="str">
+      <c r="M6" s="127" t="str">
         <f>_xlfn.CONCAT("LU Initial ", B58)</f>
         <v>LU Initial 2000</v>
       </c>
-      <c r="N6" s="124"/>
-      <c r="O6" s="125" t="str">
+      <c r="N6" s="127"/>
+      <c r="O6" s="128" t="str">
         <f>_xlfn.CONCAT("LU Final ", B59)</f>
         <v>LU Final 2024</v>
       </c>
-      <c r="P6" s="125"/>
+      <c r="P6" s="128"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="6"/>
       <c r="S6" s="7"/>
@@ -6673,7 +6720,7 @@
       <c r="AM6" s="1"/>
     </row>
     <row r="7" spans="1:39" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="27">
@@ -6773,7 +6820,7 @@
       <c r="AM7" s="1"/>
     </row>
     <row r="8" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="27">
@@ -6877,7 +6924,7 @@
       <c r="AM8" s="1"/>
     </row>
     <row r="9" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="27">
@@ -6981,7 +7028,7 @@
       <c r="AM9" s="1"/>
     </row>
     <row r="10" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B10" s="27">
@@ -7085,7 +7132,7 @@
       <c r="AM10" s="1"/>
     </row>
     <row r="11" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="27">
@@ -7189,7 +7236,7 @@
       <c r="AM11" s="1"/>
     </row>
     <row r="12" spans="1:39" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B12" s="27">
@@ -7275,7 +7322,7 @@
       <c r="AM12" s="1"/>
     </row>
     <row r="13" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="27">
@@ -7353,7 +7400,7 @@
       <c r="AM13" s="1"/>
     </row>
     <row r="14" spans="1:39" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135" t="s">
+      <c r="A14" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B14" s="27">
@@ -7429,7 +7476,7 @@
       <c r="AM14" s="1"/>
     </row>
     <row r="15" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="27">
@@ -7491,7 +7538,7 @@
       <c r="AM15" s="1"/>
     </row>
     <row r="16" spans="1:39" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="135" t="s">
+      <c r="A16" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="27">
@@ -7521,19 +7568,19 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J16" s="126" t="s">
+      <c r="J16" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="K16" s="126"/>
-      <c r="L16" s="127" t="str">
+      <c r="K16" s="129"/>
+      <c r="L16" s="130" t="str">
         <f>_xlfn.CONCAT("LU Final ", B59)</f>
         <v>LU Final 2024</v>
       </c>
-      <c r="M16" s="127"/>
-      <c r="N16" s="127"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
+      <c r="M16" s="130"/>
+      <c r="N16" s="130"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
+      <c r="Q16" s="130"/>
       <c r="R16" s="6"/>
       <c r="S16" s="7"/>
       <c r="T16" s="58" t="str">
@@ -7577,7 +7624,7 @@
       <c r="AM16" s="1"/>
     </row>
     <row r="17" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="135" t="s">
+      <c r="A17" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="27">
@@ -7607,8 +7654,8 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J17" s="126"/>
-      <c r="K17" s="126"/>
+      <c r="J17" s="129"/>
+      <c r="K17" s="129"/>
       <c r="L17" s="59" t="s">
         <v>23</v>
       </c>
@@ -7677,7 +7724,7 @@
       <c r="AM17" s="1"/>
     </row>
     <row r="18" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="27">
@@ -7707,7 +7754,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J18" s="122" t="str">
+      <c r="J18" s="131" t="str">
         <f>_xlfn.CONCAT("LU Initial ", B58)</f>
         <v>LU Initial 2000</v>
       </c>
@@ -7782,7 +7829,7 @@
       <c r="AM18" s="1"/>
     </row>
     <row r="19" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="135" t="s">
+      <c r="A19" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B19" s="27">
@@ -7812,7 +7859,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J19" s="122"/>
+      <c r="J19" s="131"/>
       <c r="K19" s="44" t="s">
         <v>28</v>
       </c>
@@ -7884,7 +7931,7 @@
       <c r="AM19" s="1"/>
     </row>
     <row r="20" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="27">
@@ -7914,7 +7961,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J20" s="122"/>
+      <c r="J20" s="131"/>
       <c r="K20" s="44" t="s">
         <v>31</v>
       </c>
@@ -7986,7 +8033,7 @@
       <c r="AM20" s="1"/>
     </row>
     <row r="21" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="27">
@@ -8016,7 +8063,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J21" s="122"/>
+      <c r="J21" s="131"/>
       <c r="K21" s="44" t="s">
         <v>34</v>
       </c>
@@ -8088,7 +8135,7 @@
       <c r="AM21" s="1"/>
     </row>
     <row r="22" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="135" t="s">
+      <c r="A22" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="27">
@@ -8118,7 +8165,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J22" s="122"/>
+      <c r="J22" s="131"/>
       <c r="K22" s="44" t="s">
         <v>37</v>
       </c>
@@ -8190,7 +8237,7 @@
       <c r="AM22" s="1"/>
     </row>
     <row r="23" spans="1:39" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="135" t="s">
+      <c r="A23" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="27">
@@ -8220,7 +8267,7 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J23" s="122"/>
+      <c r="J23" s="131"/>
       <c r="K23" s="44" t="s">
         <v>40</v>
       </c>
@@ -8274,7 +8321,7 @@
       <c r="AM23" s="1"/>
     </row>
     <row r="24" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="135" t="s">
+      <c r="A24" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B24" s="27">
@@ -8336,7 +8383,7 @@
       <c r="AM24" s="1"/>
     </row>
     <row r="25" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="135" t="s">
+      <c r="A25" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="27">
@@ -8398,7 +8445,7 @@
       <c r="AM25" s="1"/>
     </row>
     <row r="26" spans="1:39" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="135" t="s">
+      <c r="A26" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B26" s="27">
@@ -8428,19 +8475,19 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J26" s="120" t="s">
+      <c r="J26" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="120"/>
-      <c r="L26" s="128" t="str">
+      <c r="K26" s="132"/>
+      <c r="L26" s="133" t="str">
         <f>_xlfn.CONCAT("LU Final ", B59)</f>
         <v>LU Final 2024</v>
       </c>
-      <c r="M26" s="128"/>
-      <c r="N26" s="128"/>
-      <c r="O26" s="128"/>
-      <c r="P26" s="128"/>
-      <c r="Q26" s="128"/>
+      <c r="M26" s="133"/>
+      <c r="N26" s="133"/>
+      <c r="O26" s="133"/>
+      <c r="P26" s="133"/>
+      <c r="Q26" s="133"/>
       <c r="R26" s="68"/>
       <c r="S26" s="69"/>
       <c r="T26" s="34"/>
@@ -8465,7 +8512,7 @@
       <c r="AM26" s="1"/>
     </row>
     <row r="27" spans="1:39" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="135" t="s">
+      <c r="A27" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="27">
@@ -8495,8 +8542,8 @@
         <f t="shared" si="4"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J27" s="120"/>
-      <c r="K27" s="120"/>
+      <c r="J27" s="132"/>
+      <c r="K27" s="132"/>
       <c r="L27" s="59" t="s">
         <v>23</v>
       </c>
@@ -8560,7 +8607,7 @@
       <c r="AM27" s="1"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A28" s="135" t="s">
+      <c r="A28" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B28" s="27">
@@ -8570,11 +8617,26 @@
         <v>0</v>
       </c>
       <c r="D28" s="67"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="4"/>
+      <c r="E28" s="3" t="str">
+        <f t="shared" ref="E28" si="22">VLOOKUP(A28,H:I,2,FALSE)</f>
+        <v>Non-forest without changes</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f t="shared" ref="F28" si="23">LEFT(A28,1)</f>
+        <v>-</v>
+      </c>
+      <c r="G28" s="3" t="str">
+        <f t="shared" ref="G28" si="24">RIGHT(A28,1)</f>
+        <v>-</v>
+      </c>
+      <c r="H28" s="38" t="str">
+        <f t="shared" ref="H28" si="25">A28</f>
+        <v>-</v>
+      </c>
+      <c r="I28" s="4" t="str">
+        <f t="shared" ref="I28" si="26">IF( AND( G28="F", F28="F"), "Forest without changes", IF( F28="F", "Forest change to non-forest", IF(G28="F", "Non-forest change to forest", "Non-forest without changes")))</f>
+        <v>Non-forest without changes</v>
+      </c>
       <c r="J28" s="72"/>
       <c r="K28" s="72"/>
       <c r="L28" s="73"/>
@@ -8607,7 +8669,7 @@
       <c r="AM28" s="1"/>
     </row>
     <row r="29" spans="1:39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="135" t="s">
+      <c r="A29" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="27">
@@ -8618,26 +8680,26 @@
       </c>
       <c r="D29" s="67"/>
       <c r="E29" s="3" t="str">
-        <f t="shared" ref="E29:E41" si="22">VLOOKUP(A29,H:I,2,FALSE)</f>
+        <f t="shared" ref="E29:E41" si="27">VLOOKUP(A29,H:I,2,FALSE)</f>
         <v>Non-forest without changes</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f t="shared" ref="F29:F41" si="23">LEFT(A29,1)</f>
+        <f t="shared" ref="F29:F41" si="28">LEFT(A29,1)</f>
         <v>-</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f t="shared" ref="G29:G41" si="24">RIGHT(A29,1)</f>
+        <f t="shared" ref="G29:G41" si="29">RIGHT(A29,1)</f>
         <v>-</v>
       </c>
       <c r="H29" s="38" t="str">
-        <f t="shared" ref="H29:H41" si="25">A29</f>
+        <f t="shared" ref="H29:H41" si="30">A29</f>
         <v>-</v>
       </c>
       <c r="I29" s="4" t="str">
-        <f t="shared" ref="I29:I41" si="26">IF( AND( G29="F", F29="F"), "Forest without changes", IF( F29="F", "Forest change to non-forest", IF(G29="F", "Non-forest change to forest", "Non-forest without changes")))</f>
+        <f t="shared" ref="I29:I41" si="31">IF( AND( G29="F", F29="F"), "Forest without changes", IF( F29="F", "Forest change to non-forest", IF(G29="F", "Non-forest change to forest", "Non-forest without changes")))</f>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J29" s="119" t="str">
+      <c r="J29" s="134" t="str">
         <f>_xlfn.CONCAT("LU Initial ", B58)</f>
         <v>LU Initial 2000</v>
       </c>
@@ -8645,31 +8707,31 @@
         <v>23</v>
       </c>
       <c r="L29" s="78">
-        <f t="shared" ref="L29:Q34" si="27">SUMIF($A$6:$A$41,L18,$C$6:$C$42)</f>
+        <f t="shared" ref="L29:Q34" si="32">SUMIF($A$6:$A$41,L18,$C$6:$C$42)</f>
         <v>0</v>
       </c>
       <c r="M29" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N29" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O29" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P29" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q29" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R29" s="80">
-        <f t="shared" ref="R29:R35" si="28">SUM(L29:Q29)</f>
+        <f t="shared" ref="R29:R35" si="33">SUM(L29:Q29)</f>
         <v>0</v>
       </c>
       <c r="S29" s="81"/>
@@ -8722,7 +8784,7 @@
       <c r="AM29" s="1"/>
     </row>
     <row r="30" spans="1:39" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="135" t="s">
+      <c r="A30" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B30" s="27">
@@ -8733,55 +8795,55 @@
       </c>
       <c r="D30" s="67"/>
       <c r="E30" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H30" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I30" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J30" s="119"/>
+      <c r="J30" s="134"/>
       <c r="K30" s="44" t="s">
         <v>28</v>
       </c>
       <c r="L30" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M30" s="78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N30" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O30" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P30" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q30" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R30" s="80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S30" s="81"/>
@@ -8834,7 +8896,7 @@
       <c r="AM30" s="1"/>
     </row>
     <row r="31" spans="1:39" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="135" t="s">
+      <c r="A31" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B31" s="27">
@@ -8845,55 +8907,55 @@
       </c>
       <c r="D31" s="67"/>
       <c r="E31" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H31" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I31" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J31" s="119"/>
+      <c r="J31" s="134"/>
       <c r="K31" s="44" t="s">
         <v>31</v>
       </c>
       <c r="L31" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M31" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N31" s="78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O31" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P31" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q31" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R31" s="80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S31" s="81"/>
@@ -8946,7 +9008,7 @@
       <c r="AM31" s="1"/>
     </row>
     <row r="32" spans="1:39" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="135" t="s">
+      <c r="A32" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="27">
@@ -8957,55 +9019,55 @@
       </c>
       <c r="D32" s="67"/>
       <c r="E32" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H32" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I32" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J32" s="119"/>
+      <c r="J32" s="134"/>
       <c r="K32" s="44" t="s">
         <v>34</v>
       </c>
       <c r="L32" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M32" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N32" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O32" s="78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P32" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q32" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R32" s="80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S32" s="81"/>
@@ -9057,7 +9119,7 @@
       <c r="AM32" s="1"/>
     </row>
     <row r="33" spans="1:39" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="135" t="s">
+      <c r="A33" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="27">
@@ -9068,55 +9130,55 @@
       </c>
       <c r="D33" s="67"/>
       <c r="E33" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H33" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I33" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J33" s="119"/>
+      <c r="J33" s="134"/>
       <c r="K33" s="44" t="s">
         <v>37</v>
       </c>
       <c r="L33" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M33" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N33" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O33" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P33" s="78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q33" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R33" s="80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S33" s="81"/>
@@ -9150,7 +9212,7 @@
       <c r="AM33" s="1"/>
     </row>
     <row r="34" spans="1:39" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="27">
@@ -9161,55 +9223,55 @@
       </c>
       <c r="D34" s="67"/>
       <c r="E34" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H34" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I34" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J34" s="119"/>
+      <c r="J34" s="134"/>
       <c r="K34" s="44" t="s">
         <v>40</v>
       </c>
       <c r="L34" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M34" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N34" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O34" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P34" s="79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q34" s="78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R34" s="80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S34" s="81"/>
@@ -9235,7 +9297,7 @@
       <c r="AM34" s="1"/>
     </row>
     <row r="35" spans="1:39" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="135" t="s">
+      <c r="A35" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="27">
@@ -9246,23 +9308,23 @@
       </c>
       <c r="D35" s="67"/>
       <c r="E35" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H35" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I35" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="J35" s="96"/>
@@ -9271,31 +9333,31 @@
         <v>Total 2024</v>
       </c>
       <c r="L35" s="98">
-        <f t="shared" ref="L35:Q35" si="29">SUM(L29:L34)</f>
+        <f t="shared" ref="L35:Q35" si="34">SUM(L29:L34)</f>
         <v>0</v>
       </c>
       <c r="M35" s="98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="N35" s="98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O35" s="98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="P35" s="98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="Q35" s="98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="R35" s="99">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S35" s="100"/>
@@ -9321,7 +9383,7 @@
       <c r="AM35" s="1"/>
     </row>
     <row r="36" spans="1:39" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135" t="s">
+      <c r="A36" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="27">
@@ -9332,23 +9394,23 @@
       </c>
       <c r="D36" s="67"/>
       <c r="E36" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H36" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I36" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="J36" s="1"/>
@@ -9383,7 +9445,7 @@
       <c r="AM36" s="1"/>
     </row>
     <row r="37" spans="1:39" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="135" t="s">
+      <c r="A37" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="27">
@@ -9394,38 +9456,38 @@
       </c>
       <c r="D37" s="67"/>
       <c r="E37" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H37" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J37" s="120" t="s">
+      <c r="J37" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="K37" s="120"/>
-      <c r="L37" s="121" t="str">
+      <c r="K37" s="132"/>
+      <c r="L37" s="135" t="str">
         <f>_xlfn.CONCAT("LU Final ", B59)</f>
         <v>LU Final 2024</v>
       </c>
-      <c r="M37" s="121"/>
-      <c r="N37" s="121"/>
-      <c r="O37" s="121"/>
-      <c r="P37" s="121"/>
-      <c r="Q37" s="121"/>
+      <c r="M37" s="135"/>
+      <c r="N37" s="135"/>
+      <c r="O37" s="135"/>
+      <c r="P37" s="135"/>
+      <c r="Q37" s="135"/>
       <c r="R37" s="1"/>
       <c r="S37" s="11"/>
       <c r="T37" s="58" t="str">
@@ -9469,7 +9531,7 @@
       <c r="AM37" s="1"/>
     </row>
     <row r="38" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="135" t="s">
+      <c r="A38" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="27">
@@ -9480,27 +9542,27 @@
       </c>
       <c r="D38" s="67"/>
       <c r="E38" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H38" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I38" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J38" s="120"/>
-      <c r="K38" s="120"/>
+      <c r="J38" s="132"/>
+      <c r="K38" s="132"/>
       <c r="L38" s="59" t="s">
         <v>23</v>
       </c>
@@ -9569,7 +9631,7 @@
       <c r="AM38" s="1"/>
     </row>
     <row r="39" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="135" t="s">
+      <c r="A39" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="27">
@@ -9580,26 +9642,26 @@
       </c>
       <c r="D39" s="67"/>
       <c r="E39" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H39" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I39" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J39" s="122" t="str">
+      <c r="J39" s="131" t="str">
         <f>_xlfn.CONCAT("LU Initial ", B58)</f>
         <v>LU Initial 2000</v>
       </c>
@@ -9611,23 +9673,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M39" s="102" t="e">
-        <f t="shared" ref="M39:Q44" si="30">M29/$R29</f>
+        <f t="shared" ref="M39:Q44" si="35">M29/$R29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N39" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O39" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P39" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q39" s="103" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R39" s="104"/>
@@ -9680,7 +9742,7 @@
       <c r="AM39" s="1"/>
     </row>
     <row r="40" spans="1:39" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="135" t="s">
+      <c r="A40" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B40" s="27">
@@ -9691,26 +9753,26 @@
       </c>
       <c r="D40" s="67"/>
       <c r="E40" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H40" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I40" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J40" s="122"/>
+      <c r="J40" s="131"/>
       <c r="K40" s="44" t="s">
         <v>28</v>
       </c>
@@ -9719,23 +9781,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M40" s="101" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N40" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O40" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P40" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q40" s="103" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R40" s="104"/>
@@ -9788,7 +9850,7 @@
       <c r="AM40" s="1"/>
     </row>
     <row r="41" spans="1:39" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="135" t="s">
+      <c r="A41" s="118" t="s">
         <v>88</v>
       </c>
       <c r="B41" s="27">
@@ -9799,26 +9861,26 @@
       </c>
       <c r="D41" s="67"/>
       <c r="E41" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>Non-forest without changes</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="H41" s="38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="I41" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>Non-forest without changes</v>
       </c>
-      <c r="J41" s="122"/>
+      <c r="J41" s="131"/>
       <c r="K41" s="44" t="s">
         <v>31</v>
       </c>
@@ -9827,23 +9889,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M41" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N41" s="101" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O41" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P41" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q41" s="103" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R41" s="104"/>
@@ -9905,7 +9967,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="11"/>
-      <c r="J42" s="122"/>
+      <c r="J42" s="131"/>
       <c r="K42" s="44" t="s">
         <v>34</v>
       </c>
@@ -9914,23 +9976,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M42" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N42" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O42" s="101" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P42" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q42" s="103" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R42" s="104"/>
@@ -9982,7 +10044,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="11"/>
-      <c r="J43" s="122"/>
+      <c r="J43" s="131"/>
       <c r="K43" s="44" t="s">
         <v>37</v>
       </c>
@@ -9991,23 +10053,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M43" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N43" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O43" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P43" s="102" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q43" s="103" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R43" s="104"/>
@@ -10043,7 +10105,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="11"/>
-      <c r="J44" s="122"/>
+      <c r="J44" s="131"/>
       <c r="K44" s="44" t="s">
         <v>40</v>
       </c>
@@ -10052,23 +10114,23 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M44" s="109" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N44" s="109" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O44" s="109" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P44" s="109" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q44" s="110" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R44" s="104"/>
@@ -10196,17 +10258,17 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="11"/>
-      <c r="T47" s="118" t="s">
+      <c r="T47" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="U47" s="118"/>
-      <c r="V47" s="118"/>
-      <c r="W47" s="118"/>
-      <c r="X47" s="118"/>
-      <c r="Y47" s="118"/>
-      <c r="Z47" s="118"/>
-      <c r="AA47" s="118"/>
-      <c r="AB47" s="118"/>
+      <c r="U47" s="125"/>
+      <c r="V47" s="125"/>
+      <c r="W47" s="125"/>
+      <c r="X47" s="125"/>
+      <c r="Y47" s="125"/>
+      <c r="Z47" s="125"/>
+      <c r="AA47" s="125"/>
+      <c r="AB47" s="125"/>
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
       <c r="AE47" s="1"/>
@@ -10302,11 +10364,11 @@
       <c r="AM49" s="1"/>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A50" s="123" t="s">
+      <c r="A50" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="123"/>
-      <c r="C50" s="123"/>
+      <c r="B50" s="126"/>
+      <c r="C50" s="126"/>
       <c r="D50" s="1"/>
       <c r="E50" s="5"/>
       <c r="F50" s="1"/>
@@ -10427,12 +10489,12 @@
       <c r="AM52" s="1"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A53" s="118" t="s">
+      <c r="A53" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="118"/>
-      <c r="C53" s="118"/>
-      <c r="D53" s="118"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="125"/>
+      <c r="D53" s="125"/>
       <c r="E53" s="2"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -10470,10 +10532,10 @@
       <c r="AM53" s="1"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A54" s="118"/>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="125"/>
       <c r="E54" s="2"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -12602,6 +12664,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A53:D54"/>
+    <mergeCell ref="J29:J34"/>
+    <mergeCell ref="J37:K38"/>
+    <mergeCell ref="L37:Q37"/>
+    <mergeCell ref="J39:J44"/>
+    <mergeCell ref="T47:AB47"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="J18:J23"/>
+    <mergeCell ref="J26:K27"/>
+    <mergeCell ref="L26:Q26"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="J4:P4"/>
@@ -12611,20 +12687,6 @@
     <mergeCell ref="J2:S2"/>
     <mergeCell ref="T2:AB2"/>
     <mergeCell ref="AC2:AK2"/>
-    <mergeCell ref="T47:AB47"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="J16:K17"/>
-    <mergeCell ref="L16:Q16"/>
-    <mergeCell ref="J18:J23"/>
-    <mergeCell ref="J26:K27"/>
-    <mergeCell ref="L26:Q26"/>
-    <mergeCell ref="A53:D54"/>
-    <mergeCell ref="J29:J34"/>
-    <mergeCell ref="J37:K38"/>
-    <mergeCell ref="L37:Q37"/>
-    <mergeCell ref="J39:J44"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:A41">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">

</xml_diff>